<commit_message>
AIP-386 AIP-454 Test Data File
</commit_message>
<xml_diff>
--- a/Carrick_AutomatedTest/Carrick_Automation/TestData/CAM_736.xlsx
+++ b/Carrick_AutomatedTest/Carrick_Automation/TestData/CAM_736.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3673A62-39CE-48CF-8F29-09E58736E1E7}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF1D5F4B-B501-4AF1-A867-0A83053183CE}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20610" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="44">
   <si>
     <t>IDM+18</t>
   </si>
@@ -122,6 +122,36 @@
   </si>
   <si>
     <t>TimeMasterClock_Setting</t>
+  </si>
+  <si>
+    <t>UDPPortNumber1</t>
+  </si>
+  <si>
+    <t>1025</t>
+  </si>
+  <si>
+    <t>GroupMaskID1</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>Compatibility1</t>
+  </si>
+  <si>
+    <t>UDPPortNumber2</t>
+  </si>
+  <si>
+    <t>GroupMaskID2</t>
+  </si>
+  <si>
+    <t>Compatibility2</t>
+  </si>
+  <si>
+    <t>Delay</t>
+  </si>
+  <si>
+    <t>NumberofTimes</t>
   </si>
 </sst>
 </file>
@@ -440,10 +470,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U3"/>
+  <dimension ref="A1:AC3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="T3" sqref="T3"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -457,13 +487,13 @@
     <col min="7" max="10" width="14.7109375" customWidth="1"/>
     <col min="11" max="11" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="20" max="21" width="28" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="26" max="27" width="28" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -504,31 +534,55 @@
         <v>23</v>
       </c>
       <c r="N1" t="s">
+        <v>34</v>
+      </c>
+      <c r="O1" t="s">
+        <v>36</v>
+      </c>
+      <c r="P1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q1" t="s">
         <v>24</v>
       </c>
-      <c r="O1" t="s">
+      <c r="R1" t="s">
         <v>25</v>
       </c>
-      <c r="P1" t="s">
+      <c r="S1" t="s">
         <v>26</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="T1" t="s">
+        <v>39</v>
+      </c>
+      <c r="U1" t="s">
+        <v>40</v>
+      </c>
+      <c r="V1" t="s">
+        <v>41</v>
+      </c>
+      <c r="W1" t="s">
         <v>28</v>
       </c>
-      <c r="R1" t="s">
+      <c r="X1" t="s">
         <v>29</v>
       </c>
-      <c r="S1" t="s">
+      <c r="Y1" t="s">
         <v>33</v>
       </c>
-      <c r="T1" t="s">
+      <c r="Z1" t="s">
         <v>30</v>
       </c>
-      <c r="U1" t="s">
+      <c r="AA1" t="s">
         <v>31</v>
       </c>
+      <c r="AB1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>43</v>
+      </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -569,31 +623,49 @@
         <v>7</v>
       </c>
       <c r="N2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="R2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="S2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="T2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="W2" t="s">
         <v>4</v>
       </c>
-      <c r="R2" t="s">
+      <c r="X2" t="s">
         <v>14</v>
       </c>
-      <c r="S2" t="s">
+      <c r="Y2" t="s">
         <v>27</v>
       </c>
-      <c r="T2" t="s">
+      <c r="Z2" t="s">
         <v>5</v>
       </c>
-      <c r="U2" t="s">
+      <c r="AA2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -634,27 +706,45 @@
         <v>7</v>
       </c>
       <c r="N3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="O3" s="1" t="s">
+      <c r="R3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="P3" s="1" t="s">
+      <c r="S3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="T3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="W3" t="s">
         <v>14</v>
       </c>
-      <c r="R3" t="s">
+      <c r="X3" t="s">
         <v>4</v>
       </c>
-      <c r="S3" t="s">
+      <c r="Y3" t="s">
         <v>27</v>
       </c>
-      <c r="T3" t="s">
+      <c r="Z3" t="s">
         <v>15</v>
       </c>
-      <c r="U3" t="s">
+      <c r="AA3" t="s">
         <v>32</v>
       </c>
     </row>

</xml_diff>

<commit_message>
AIP-386 AIP-454 Updated Test Data File
</commit_message>
<xml_diff>
--- a/Carrick_AutomatedTest/Carrick_Automation/TestData/CAM_736.xlsx
+++ b/Carrick_AutomatedTest/Carrick_Automation/TestData/CAM_736.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF1D5F4B-B501-4AF1-A867-0A83053183CE}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2DE254E-D407-410B-89FD-5E47468660F8}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="47">
   <si>
     <t>IDM+18</t>
   </si>
@@ -46,9 +46,6 @@
     <t>30000</t>
   </si>
   <si>
-    <t>1500</t>
-  </si>
-  <si>
     <t>DeviceName1</t>
   </si>
   <si>
@@ -133,9 +130,6 @@
     <t>GroupMaskID1</t>
   </si>
   <si>
-    <t>13</t>
-  </si>
-  <si>
     <t>Compatibility1</t>
   </si>
   <si>
@@ -148,10 +142,25 @@
     <t>Compatibility2</t>
   </si>
   <si>
-    <t>Delay</t>
-  </si>
-  <si>
-    <t>NumberofTimes</t>
+    <t>2000</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>NoOfManualTrigger</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>5000</t>
+  </si>
+  <si>
+    <t>ExpectedRecordLength</t>
   </si>
 </sst>
 </file>
@@ -470,10 +479,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AC3"/>
+  <dimension ref="A1:AC2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="R2" sqref="R2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -491,6 +500,7 @@
     <col min="24" max="24" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="26" max="27" width="28" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="18.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.25">
@@ -501,85 +511,85 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
         <v>9</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>10</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>11</v>
       </c>
-      <c r="F1" t="s">
-        <v>12</v>
-      </c>
       <c r="G1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" t="s">
         <v>17</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>18</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>19</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>20</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>21</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>22</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O1" t="s">
+        <v>35</v>
+      </c>
+      <c r="P1" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q1" t="s">
         <v>23</v>
       </c>
-      <c r="N1" t="s">
-        <v>34</v>
-      </c>
-      <c r="O1" t="s">
-        <v>36</v>
-      </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
+        <v>24</v>
+      </c>
+      <c r="S1" t="s">
+        <v>25</v>
+      </c>
+      <c r="T1" t="s">
+        <v>37</v>
+      </c>
+      <c r="U1" t="s">
         <v>38</v>
       </c>
-      <c r="Q1" t="s">
-        <v>24</v>
-      </c>
-      <c r="R1" t="s">
-        <v>25</v>
-      </c>
-      <c r="S1" t="s">
-        <v>26</v>
-      </c>
-      <c r="T1" t="s">
+      <c r="V1" t="s">
         <v>39</v>
       </c>
-      <c r="U1" t="s">
-        <v>40</v>
-      </c>
-      <c r="V1" t="s">
-        <v>41</v>
-      </c>
       <c r="W1" t="s">
+        <v>27</v>
+      </c>
+      <c r="X1" t="s">
         <v>28</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Z1" t="s">
         <v>29</v>
       </c>
-      <c r="Y1" t="s">
-        <v>33</v>
-      </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>30</v>
       </c>
-      <c r="AA1" t="s">
-        <v>31</v>
-      </c>
       <c r="AB1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AC1" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.25">
@@ -599,153 +609,76 @@
         <v>5</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
         <v>13</v>
-      </c>
-      <c r="G2" t="s">
-        <v>14</v>
       </c>
       <c r="H2" t="s">
         <v>0</v>
       </c>
       <c r="I2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>6</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="M2" s="1" t="s">
         <v>7</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="Q2" s="1" t="s">
         <v>6</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>8</v>
+        <v>45</v>
       </c>
       <c r="S2" s="1" t="s">
         <v>7</v>
       </c>
       <c r="T2" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="U2" s="1" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="V2" s="1" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="W2" t="s">
         <v>4</v>
       </c>
       <c r="X2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="Y2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="Z2" t="s">
         <v>5</v>
       </c>
       <c r="AA2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3" t="s">
-        <v>0</v>
-      </c>
-      <c r="I3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="M3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AC2" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="R3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="S3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="T3" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="U3" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="V3" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="W3" t="s">
-        <v>14</v>
-      </c>
-      <c r="X3" t="s">
-        <v>4</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>27</v>
-      </c>
-      <c r="Z3" t="s">
-        <v>15</v>
-      </c>
-      <c r="AA3" t="s">
-        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
AIP-392 AIP-466 Updated Test Data for 2 Iteration and for group mask
</commit_message>
<xml_diff>
--- a/Carrick_AutomatedTest/Carrick_Automation/TestData/CAM_736.xlsx
+++ b/Carrick_AutomatedTest/Carrick_Automation/TestData/CAM_736.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2DE254E-D407-410B-89FD-5E47468660F8}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{504FBF37-2CE8-4E76-8A87-3AD5BF183ABA}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="52">
   <si>
     <t>IDM+18</t>
   </si>
@@ -127,18 +127,12 @@
     <t>1025</t>
   </si>
   <si>
-    <t>GroupMaskID1</t>
-  </si>
-  <si>
     <t>Compatibility1</t>
   </si>
   <si>
     <t>UDPPortNumber2</t>
   </si>
   <si>
-    <t>GroupMaskID2</t>
-  </si>
-  <si>
     <t>Compatibility2</t>
   </si>
   <si>
@@ -154,13 +148,34 @@
     <t>NoOfManualTrigger</t>
   </si>
   <si>
-    <t>15</t>
-  </si>
-  <si>
     <t>5000</t>
   </si>
   <si>
     <t>ExpectedRecordLength</t>
+  </si>
+  <si>
+    <t>Grp1_GroupMaskID1</t>
+  </si>
+  <si>
+    <t>Grp2_GroupMaskID1</t>
+  </si>
+  <si>
+    <t>Grp3_GroupMaskID1</t>
+  </si>
+  <si>
+    <t>Grp4_GroupMaskID1</t>
+  </si>
+  <si>
+    <t>Grp1_GroupMaskID2</t>
+  </si>
+  <si>
+    <t>Grp2_GroupMaskID2</t>
+  </si>
+  <si>
+    <t>Grp3_GroupMaskID2</t>
+  </si>
+  <si>
+    <t>Grp4_GroupMaskID2</t>
   </si>
 </sst>
 </file>
@@ -479,31 +494,44 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AC2"/>
+  <dimension ref="A1:AI3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="AF3" sqref="AF3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="10" width="14.7109375" customWidth="1"/>
-    <col min="11" max="11" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="26" max="27" width="28" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="17" width="16.85546875" customWidth="1"/>
+    <col min="18" max="18" width="14" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="14" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="26" max="27" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="28" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="28" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -547,52 +575,70 @@
         <v>33</v>
       </c>
       <c r="O1" t="s">
+        <v>44</v>
+      </c>
+      <c r="P1" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>46</v>
+      </c>
+      <c r="R1" t="s">
+        <v>47</v>
+      </c>
+      <c r="S1" t="s">
         <v>35</v>
       </c>
-      <c r="P1" t="s">
+      <c r="T1" t="s">
+        <v>23</v>
+      </c>
+      <c r="U1" t="s">
+        <v>24</v>
+      </c>
+      <c r="V1" t="s">
+        <v>25</v>
+      </c>
+      <c r="W1" t="s">
         <v>36</v>
       </c>
-      <c r="Q1" t="s">
-        <v>23</v>
-      </c>
-      <c r="R1" t="s">
-        <v>24</v>
-      </c>
-      <c r="S1" t="s">
-        <v>25</v>
-      </c>
-      <c r="T1" t="s">
+      <c r="X1" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>49</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AB1" t="s">
         <v>37</v>
       </c>
-      <c r="U1" t="s">
-        <v>38</v>
-      </c>
-      <c r="V1" t="s">
-        <v>39</v>
-      </c>
-      <c r="W1" t="s">
+      <c r="AC1" t="s">
         <v>27</v>
       </c>
-      <c r="X1" t="s">
+      <c r="AD1" t="s">
         <v>28</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AE1" t="s">
         <v>32</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AF1" t="s">
         <v>29</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AG1" t="s">
         <v>30</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AH1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AI1" t="s">
         <v>43</v>
       </c>
-      <c r="AC1" t="s">
-        <v>46</v>
-      </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -627,7 +673,7 @@
         <v>6</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="M2" s="1" t="s">
         <v>7</v>
@@ -636,48 +682,173 @@
         <v>34</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="P2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="U2" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="V2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>4</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>26</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>5</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>31</v>
+      </c>
+      <c r="AH2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AI2" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" t="s">
+        <v>0</v>
+      </c>
+      <c r="I3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="R2" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="S2" s="1" t="s">
+      <c r="L3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="M3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="T2" s="1" t="s">
+      <c r="N3" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="U2" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="V2" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="W2" t="s">
+      <c r="O3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="X3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD3" t="s">
         <v>4</v>
       </c>
-      <c r="X2" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y2" t="s">
+      <c r="AE3" t="s">
         <v>26</v>
       </c>
-      <c r="Z2" t="s">
-        <v>5</v>
-      </c>
-      <c r="AA2" t="s">
+      <c r="AF3" t="s">
+        <v>14</v>
+      </c>
+      <c r="AG3" t="s">
         <v>31</v>
       </c>
-      <c r="AB2" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="AC2" s="1" t="s">
+      <c r="AH3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AI3" s="1" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>